<commit_message>
Changed uploading files button and resetting
</commit_message>
<xml_diff>
--- a/uploaded_data.xlsx
+++ b/uploaded_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dancocapitalltd.sharepoint.com/sites/DANCOOPERATIONS/Shared Documents/DANCO PRODUCTION/OKR Q3  Supporting documents/Power of one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1539" documentId="8_{024FBB20-08A9-44E7-B8F8-F491183F506D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31688600-0F1F-4F0D-AF77-3E6CCD90C6F5}"/>
+  <xr:revisionPtr revIDLastSave="1543" documentId="8_{024FBB20-08A9-44E7-B8F8-F491183F506D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2693926-363A-4BEA-BCAF-802D4B93A101}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="6" activeTab="2" xr2:uid="{473E9D55-B832-414D-9AC3-A1EA3E177109}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="6" activeTab="6" xr2:uid="{473E9D55-B832-414D-9AC3-A1EA3E177109}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Job Details'!$A$2:$AB$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'POWERBI SUMMARY'!$A$1:$J$109</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$2:$Z$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'POWERBI SUMMARY'!$A$1:$J$109</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -341,7 +341,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1056,13 +1056,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1074,14 +1077,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1744,6 +1744,10 @@
 </externalLink>
 </file>
 
+<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
+<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2068,7 +2072,7 @@
       <selection pane="topRight" activeCell="U3" sqref="U3:Z29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="2" customWidth="1"/>
@@ -2099,7 +2103,7 @@
     <col min="27" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="6" customFormat="1">
+    <row r="1" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="7"/>
       <c r="C1" s="13" t="s">
@@ -2175,7 +2179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="6" customFormat="1">
+    <row r="2" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
@@ -2255,7 +2259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="1" customFormat="1">
+    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -2336,7 +2340,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="1" customFormat="1">
+    <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -2417,7 +2421,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="1" customFormat="1">
+    <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="1" customFormat="1">
+    <row r="6" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2544,7 +2548,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="1" customFormat="1">
+    <row r="7" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -2644,7 +2648,7 @@
         <v>0.10714285714285714</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="1" customFormat="1">
+    <row r="8" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -2681,7 +2685,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="1" customFormat="1">
+    <row r="9" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2763,7 +2767,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="1" customFormat="1">
+    <row r="10" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -2853,7 +2857,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="1" customFormat="1">
+    <row r="11" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -2890,7 +2894,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="1" customFormat="1">
+    <row r="12" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -2974,7 +2978,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="1" customFormat="1">
+    <row r="13" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -3058,7 +3062,7 @@
         <v>7.2542145513532996E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="1" customFormat="1">
+    <row r="14" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -3092,7 +3096,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="1" customFormat="1">
+    <row r="15" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -3166,7 +3170,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="1" customFormat="1">
+    <row r="16" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -3240,7 +3244,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="1" customFormat="1">
+    <row r="17" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -3273,7 +3277,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="1" customFormat="1">
+    <row r="18" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -3347,7 +3351,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:26" s="1" customFormat="1">
+    <row r="19" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -3421,7 +3425,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:26" s="1" customFormat="1">
+    <row r="20" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -3454,7 +3458,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:26" s="1" customFormat="1">
+    <row r="21" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -3518,7 +3522,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="1" customFormat="1">
+    <row r="22" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -3582,7 +3586,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:26" s="1" customFormat="1">
+    <row r="23" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -3615,7 +3619,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="1" customFormat="1">
+    <row r="24" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -3673,7 +3677,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:26" s="1" customFormat="1">
+    <row r="25" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -3731,7 +3735,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:26" s="1" customFormat="1">
+    <row r="26" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -3764,7 +3768,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:26" s="1" customFormat="1">
+    <row r="27" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -3828,7 +3832,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:26" s="1" customFormat="1">
+    <row r="28" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -3892,7 +3896,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:26" s="47" customFormat="1" ht="15.75" thickBot="1">
+    <row r="29" spans="1:26" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -3925,7 +3929,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:26" s="25" customFormat="1" ht="15.75" thickBot="1">
+    <row r="30" spans="1:26" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>40</v>
       </c>
@@ -4002,9 +4006,9 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5" t="s">
@@ -4026,7 +4030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -4052,7 +4056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4082,7 +4086,7 @@
         <v>0.11507936507936503</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -4120,12 +4124,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E70EFF-3DD1-4F63-AB5D-039692A2D1E2}">
   <dimension ref="A1:AB94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="2" customWidth="1"/>
@@ -4158,7 +4162,7 @@
     <col min="29" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1">
+    <row r="1" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -4236,7 +4240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1">
+    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>41</v>
       </c>
@@ -4322,7 +4326,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1">
+    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20">
         <v>45931</v>
       </c>
@@ -4396,7 +4400,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1">
+    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20">
         <v>45931</v>
       </c>
@@ -4478,7 +4482,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1">
+    <row r="5" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20">
         <v>45931</v>
       </c>
@@ -4552,7 +4556,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1">
+    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20">
         <v>45931</v>
       </c>
@@ -4627,7 +4631,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="1" customFormat="1">
+    <row r="7" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20">
         <v>45931</v>
       </c>
@@ -4702,7 +4706,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="1" customFormat="1">
+    <row r="8" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20">
         <v>45931</v>
       </c>
@@ -4777,7 +4781,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="1" customFormat="1">
+    <row r="9" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20">
         <v>45932</v>
       </c>
@@ -4851,7 +4855,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:28" s="1" customFormat="1">
+    <row r="10" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20">
         <v>45932</v>
       </c>
@@ -4925,7 +4929,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:28" s="1" customFormat="1">
+    <row r="11" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="20">
         <v>45932</v>
       </c>
@@ -5000,7 +5004,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="1" customFormat="1">
+    <row r="12" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20">
         <v>45933</v>
       </c>
@@ -5074,7 +5078,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="1" customFormat="1">
+    <row r="13" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="20">
         <v>45933</v>
       </c>
@@ -5148,7 +5152,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:28" s="1" customFormat="1">
+    <row r="14" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20">
         <v>45933</v>
       </c>
@@ -5222,7 +5226,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1">
+    <row r="15" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20">
         <v>45933</v>
       </c>
@@ -5296,7 +5300,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="1" customFormat="1">
+    <row r="16" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="20">
         <v>45933</v>
       </c>
@@ -5370,7 +5374,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="2:28" s="1" customFormat="1">
+    <row r="17" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20">
         <v>45933</v>
       </c>
@@ -5445,7 +5449,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="2:28" s="1" customFormat="1">
+    <row r="18" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="20">
         <v>45934</v>
       </c>
@@ -5519,7 +5523,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="2:28" s="1" customFormat="1">
+    <row r="19" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="20">
         <v>45934</v>
       </c>
@@ -5594,7 +5598,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="2:28" s="1" customFormat="1" ht="15.75" thickBot="1">
+    <row r="20" spans="2:28" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="20">
         <v>45934</v>
       </c>
@@ -5668,7 +5672,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="2:28" s="1" customFormat="1">
+    <row r="21" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="20">
         <v>45936</v>
       </c>
@@ -5745,7 +5749,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="2:28" s="1" customFormat="1">
+    <row r="22" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="20">
         <v>45936</v>
       </c>
@@ -5819,7 +5823,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="2:28" s="1" customFormat="1">
+    <row r="23" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20">
         <v>45936</v>
       </c>
@@ -5892,7 +5896,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:28" s="1" customFormat="1">
+    <row r="24" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="20">
         <v>45936</v>
       </c>
@@ -5966,7 +5970,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="2:28" s="1" customFormat="1">
+    <row r="25" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="20">
         <v>45937</v>
       </c>
@@ -6041,7 +6045,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="2:28" s="1" customFormat="1">
+    <row r="26" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20">
         <v>45937</v>
       </c>
@@ -6115,7 +6119,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="2:28" s="1" customFormat="1">
+    <row r="27" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="20">
         <v>45937</v>
       </c>
@@ -6190,7 +6194,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="2:28" s="1" customFormat="1">
+    <row r="28" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="20">
         <v>45938</v>
       </c>
@@ -6265,7 +6269,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:28" s="1" customFormat="1">
+    <row r="29" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20">
         <v>45938</v>
       </c>
@@ -6340,7 +6344,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:28" s="1" customFormat="1">
+    <row r="30" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20">
         <v>45938</v>
       </c>
@@ -6414,7 +6418,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="2:28" s="1" customFormat="1">
+    <row r="31" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="20">
         <v>45938</v>
       </c>
@@ -6489,7 +6493,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:28" s="1" customFormat="1">
+    <row r="32" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="20">
         <v>45938</v>
       </c>
@@ -6564,7 +6568,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="2:28" s="1" customFormat="1">
+    <row r="33" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="20">
         <v>45938</v>
       </c>
@@ -6639,7 +6643,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="2:28" s="1" customFormat="1">
+    <row r="34" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="20">
         <v>45938</v>
       </c>
@@ -6714,7 +6718,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="2:28" s="1" customFormat="1">
+    <row r="35" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="20">
         <v>45939</v>
       </c>
@@ -6788,7 +6792,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="2:28" s="1" customFormat="1">
+    <row r="36" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="20">
         <v>45939</v>
       </c>
@@ -6863,7 +6867,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="2:28" s="1" customFormat="1">
+    <row r="37" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="20">
         <v>45939</v>
       </c>
@@ -6946,7 +6950,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="2:28" s="1" customFormat="1">
+    <row r="38" spans="2:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="20">
         <v>45939</v>
       </c>
@@ -7021,7 +7025,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="2:28" s="23" customFormat="1">
+    <row r="39" spans="2:28" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="20">
         <v>45940</v>
       </c>
@@ -7096,7 +7100,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="2:28">
+    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B40" s="20">
         <v>45940</v>
       </c>
@@ -7165,7 +7169,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="2:28">
+    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B41" s="20">
         <v>45940</v>
       </c>
@@ -7228,7 +7232,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="2:28">
+    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B42" s="20">
         <v>45940</v>
       </c>
@@ -7291,7 +7295,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="2:28">
+    <row r="43" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B43" s="20">
         <v>45940</v>
       </c>
@@ -7371,7 +7375,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="2:28">
+    <row r="44" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B44" s="20">
         <v>45941</v>
       </c>
@@ -7440,7 +7444,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="2:28">
+    <row r="45" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B45" s="20">
         <v>45941</v>
       </c>
@@ -7509,7 +7513,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="2:28">
+    <row r="46" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B46" s="20">
         <v>45941</v>
       </c>
@@ -7572,7 +7576,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="2:28">
+    <row r="47" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B47" s="20">
         <v>45941</v>
       </c>
@@ -7635,7 +7639,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="2:28">
+    <row r="48" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B48" s="20">
         <v>45941</v>
       </c>
@@ -7698,7 +7702,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="2:28">
+    <row r="49" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B49" s="20">
         <v>45941</v>
       </c>
@@ -7768,7 +7772,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="2:28">
+    <row r="50" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B50" s="20">
         <v>45941</v>
       </c>
@@ -7838,7 +7842,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="51" spans="2:28">
+    <row r="51" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B51" s="20">
         <v>45943</v>
       </c>
@@ -7917,7 +7921,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="52" spans="2:28">
+    <row r="52" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B52" s="20">
         <v>45943</v>
       </c>
@@ -7986,7 +7990,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="2:28">
+    <row r="53" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B53" s="20">
         <v>45943</v>
       </c>
@@ -8056,7 +8060,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="2:28">
+    <row r="54" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B54" s="20">
         <v>45943</v>
       </c>
@@ -8126,7 +8130,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="2:28">
+    <row r="55" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B55" s="20">
         <v>45944</v>
       </c>
@@ -8205,7 +8209,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="2:28">
+    <row r="56" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B56" s="20">
         <v>45944</v>
       </c>
@@ -8275,7 +8279,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="2:28">
+    <row r="57" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B57" s="20">
         <v>45944</v>
       </c>
@@ -8345,7 +8349,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="2:28">
+    <row r="58" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B58" s="20">
         <v>45944</v>
       </c>
@@ -8415,7 +8419,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="2:28">
+    <row r="59" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B59" s="20">
         <v>45944</v>
       </c>
@@ -8485,7 +8489,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="2:28">
+    <row r="60" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B60" s="20">
         <v>45944</v>
       </c>
@@ -8555,7 +8559,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="2:28">
+    <row r="61" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B61" s="20">
         <v>45945</v>
       </c>
@@ -8625,7 +8629,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="62" spans="2:28">
+    <row r="62" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B62" s="20">
         <v>45945</v>
       </c>
@@ -8695,7 +8699,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="63" spans="2:28">
+    <row r="63" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B63" s="20">
         <v>45945</v>
       </c>
@@ -8765,7 +8769,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="64" spans="2:28">
+    <row r="64" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B64" s="20">
         <v>45945</v>
       </c>
@@ -8835,7 +8839,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="2:28">
+    <row r="65" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B65" s="20">
         <v>45945</v>
       </c>
@@ -8904,7 +8908,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="2:28">
+    <row r="66" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B66" s="20">
         <v>45945</v>
       </c>
@@ -8973,7 +8977,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="2:28">
+    <row r="67" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B67" s="20">
         <v>45945</v>
       </c>
@@ -9042,7 +9046,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="2:28">
+    <row r="68" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B68" s="20">
         <v>45945</v>
       </c>
@@ -9112,7 +9116,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="69" spans="2:28">
+    <row r="69" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B69" s="20">
         <v>45945</v>
       </c>
@@ -9182,7 +9186,7 @@
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="70" spans="2:28">
+    <row r="70" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B70" s="20">
         <v>45946</v>
       </c>
@@ -9251,7 +9255,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="2:28">
+    <row r="71" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B71" s="20">
         <v>45946</v>
       </c>
@@ -9321,7 +9325,7 @@
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="72" spans="2:28">
+    <row r="72" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B72" s="20">
         <v>45946</v>
       </c>
@@ -9391,7 +9395,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="73" spans="2:28">
+    <row r="73" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B73" s="20">
         <v>45946</v>
       </c>
@@ -9461,7 +9465,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="74" spans="2:28">
+    <row r="74" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B74" s="20">
         <v>45948</v>
       </c>
@@ -9530,7 +9534,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="75" spans="2:28">
+    <row r="75" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B75" s="20">
         <v>45948</v>
       </c>
@@ -9599,7 +9603,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="2:28">
+    <row r="76" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B76" s="20">
         <v>45948</v>
       </c>
@@ -9668,7 +9672,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="2:28">
+    <row r="77" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B77" s="20">
         <v>45948</v>
       </c>
@@ -9738,7 +9742,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="2:28">
+    <row r="78" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B78" s="20">
         <v>45948</v>
       </c>
@@ -9808,7 +9812,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="79" spans="2:28">
+    <row r="79" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B79" s="20">
         <v>45951</v>
       </c>
@@ -9877,7 +9881,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="80" spans="2:28">
+    <row r="80" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B80" s="20">
         <v>45951</v>
       </c>
@@ -9947,7 +9951,7 @@
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:28">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B81" s="20">
         <v>45951</v>
       </c>
@@ -10017,7 +10021,7 @@
         <v>0.10714285714285714</v>
       </c>
     </row>
-    <row r="82" spans="1:28">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B82" s="20">
         <v>45951</v>
       </c>
@@ -10087,7 +10091,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="83" spans="1:28">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B83" s="20">
         <v>45951</v>
       </c>
@@ -10157,7 +10161,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="84" spans="1:28">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B84" s="20">
         <v>45951</v>
       </c>
@@ -10227,7 +10231,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="85" spans="1:28">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B85" s="20">
         <v>45951</v>
       </c>
@@ -10297,7 +10301,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="86" spans="1:28">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D86" s="23" t="s">
         <v>13</v>
       </c>
@@ -10351,7 +10355,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="87" spans="1:28">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D87" s="23" t="s">
         <v>13</v>
       </c>
@@ -10405,7 +10409,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="88" spans="1:28">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D88" s="23" t="s">
         <v>13</v>
       </c>
@@ -10459,7 +10463,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="89" spans="1:28">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D89" s="23" t="s">
         <v>13</v>
       </c>
@@ -10513,7 +10517,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="90" spans="1:28">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D90" s="23" t="s">
         <v>13</v>
       </c>
@@ -10567,7 +10571,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="91" spans="1:28">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D91" s="23" t="s">
         <v>13</v>
       </c>
@@ -10621,7 +10625,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="92" spans="1:28">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D92" s="23" t="s">
         <v>13</v>
       </c>
@@ -10675,7 +10679,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="15.75" thickBot="1">
+    <row r="93" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D93" s="23" t="s">
         <v>13</v>
       </c>
@@ -10729,7 +10733,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="94" spans="1:28" s="27" customFormat="1" ht="15.75" thickBot="1">
+    <row r="94" spans="1:28" s="27" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="26"/>
       <c r="C94" s="27" t="s">
         <v>40</v>
@@ -10807,12 +10811,12 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" s="1" customFormat="1">
+    <row r="1" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="20">
         <v>45930</v>
       </c>
@@ -10876,7 +10880,7 @@
       </c>
       <c r="W1" s="32"/>
     </row>
-    <row r="2" spans="2:23" s="1" customFormat="1">
+    <row r="2" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="20">
         <v>45930</v>
       </c>
@@ -10944,7 +10948,7 @@
       </c>
       <c r="W2" s="32"/>
     </row>
-    <row r="3" spans="2:23" s="1" customFormat="1">
+    <row r="3" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20">
         <v>45930</v>
       </c>
@@ -11003,7 +11007,7 @@
       </c>
       <c r="W3" s="32"/>
     </row>
-    <row r="4" spans="2:23" s="1" customFormat="1">
+    <row r="4" spans="2:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20">
         <v>45930</v>
       </c>
@@ -11078,7 +11082,7 @@
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="5" width="11.85546875" customWidth="1"/>
@@ -11088,7 +11092,7 @@
     <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="22.9" customHeight="1">
+    <row r="3" spans="2:11" ht="22.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="69" t="s">
         <v>43</v>
       </c>
@@ -11102,7 +11106,7 @@
       <c r="J3" s="69"/>
       <c r="K3" s="69"/>
     </row>
-    <row r="4" spans="2:11" ht="32.450000000000003" customHeight="1">
+    <row r="4" spans="2:11" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="44" t="s">
         <v>44</v>
       </c>
@@ -11126,7 +11130,7 @@
       </c>
       <c r="K4" s="71"/>
     </row>
-    <row r="5" spans="2:11" ht="32.450000000000003" customHeight="1">
+    <row r="5" spans="2:11" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
       <c r="D5" s="44" t="s">
@@ -11154,7 +11158,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1</v>
       </c>
@@ -11190,7 +11194,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -11226,7 +11230,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>3</v>
       </c>
@@ -11254,7 +11258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>4</v>
       </c>
@@ -11290,7 +11294,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -11326,7 +11330,7 @@
         <v>214.5</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>6</v>
       </c>
@@ -11354,7 +11358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>7</v>
       </c>
@@ -11390,7 +11394,7 @@
         <v>214.5</v>
       </c>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>8</v>
       </c>
@@ -11426,7 +11430,7 @@
         <v>214.5</v>
       </c>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>9</v>
       </c>
@@ -11454,7 +11458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>10</v>
       </c>
@@ -11490,7 +11494,7 @@
         <v>214.5</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>11</v>
       </c>
@@ -11526,7 +11530,7 @@
         <v>214.5</v>
       </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>12</v>
       </c>
@@ -11554,7 +11558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>13</v>
       </c>
@@ -11590,7 +11594,7 @@
         <v>214.5</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>14</v>
       </c>
@@ -11626,7 +11630,7 @@
         <v>214.5</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>15</v>
       </c>
@@ -11654,7 +11658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>16</v>
       </c>
@@ -11690,7 +11694,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>17</v>
       </c>
@@ -11726,7 +11730,7 @@
         <v>225.5</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>18</v>
       </c>
@@ -11751,7 +11755,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>19</v>
       </c>
@@ -11782,7 +11786,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>20</v>
       </c>
@@ -11813,7 +11817,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>21</v>
       </c>
@@ -11844,7 +11848,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>22</v>
       </c>
@@ -11875,7 +11879,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>23</v>
       </c>
@@ -11906,7 +11910,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>24</v>
       </c>
@@ -11962,7 +11966,7 @@
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
@@ -11970,408 +11974,402 @@
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1">
-      <c r="A1" s="72" t="s">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="74" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="41"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="77"/>
-    </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1">
+      <c r="C3" s="76"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="78"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="42"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-    </row>
-    <row r="5" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A5" s="74" t="s">
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+    </row>
+    <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-    </row>
-    <row r="6" spans="1:7" ht="21" customHeight="1">
-      <c r="A6" s="74" t="s">
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+    </row>
+    <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-    </row>
-    <row r="7" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A7" s="74" t="s">
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+    </row>
+    <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="74" t="s">
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="72"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A10" s="74" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-    </row>
-    <row r="11" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A11" s="74" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="73"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-    </row>
-    <row r="13" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A13" s="74" t="s">
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="72"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+    </row>
+    <row r="13" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-    </row>
-    <row r="14" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A14" s="74" t="s">
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+    </row>
+    <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-    </row>
-    <row r="15" spans="1:7" ht="21" customHeight="1">
-      <c r="A15" s="74" t="s">
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+    </row>
+    <row r="15" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-    </row>
-    <row r="17" spans="1:7" ht="21" customHeight="1">
-      <c r="A17" s="74" t="s">
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="72"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+    </row>
+    <row r="17" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-    </row>
-    <row r="18" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A18" s="74" t="s">
+      <c r="B17" s="79"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+    </row>
+    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="74"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-    </row>
-    <row r="19" spans="1:7" ht="21" customHeight="1">
-      <c r="A19" s="74" t="s">
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+    </row>
+    <row r="19" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-    </row>
-    <row r="21" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A21" s="74" t="s">
+      <c r="B19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="72"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
+    </row>
+    <row r="21" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-    </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1">
-      <c r="A22" s="74" t="s">
+      <c r="B21" s="79"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+    </row>
+    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-    </row>
-    <row r="23" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A23" s="74" t="s">
+      <c r="B22" s="79"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="79"/>
+    </row>
+    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="73"/>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-    </row>
-    <row r="25" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A25" s="74" t="s">
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="72"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+    </row>
+    <row r="25" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-    </row>
-    <row r="26" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A26" s="74" t="s">
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+    </row>
+    <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-    </row>
-    <row r="27" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A27" s="74" t="s">
+      <c r="B26" s="79"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+    </row>
+    <row r="27" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-    </row>
-    <row r="28" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A28" s="75"/>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="77"/>
-    </row>
-    <row r="29" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A29" s="75"/>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="77"/>
-    </row>
-    <row r="30" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A30" s="75"/>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="77"/>
-    </row>
-    <row r="31" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A31" s="75"/>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="77"/>
-    </row>
-    <row r="32" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A32" s="78" t="s">
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+    </row>
+    <row r="28" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="76"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="78"/>
+    </row>
+    <row r="29" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="76"/>
+      <c r="B29" s="77"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="78"/>
+    </row>
+    <row r="30" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="76"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="78"/>
+    </row>
+    <row r="31" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="76"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="78"/>
+    </row>
+    <row r="32" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="79"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="79"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="80"/>
-    </row>
-    <row r="33" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A33" s="78" t="s">
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="75"/>
+    </row>
+    <row r="33" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="79"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="80"/>
-    </row>
-    <row r="34" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A34" s="75"/>
-      <c r="B34" s="76"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="77"/>
-    </row>
-    <row r="35" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A35" s="75"/>
-      <c r="B35" s="76"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="77"/>
-    </row>
-    <row r="36" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A36" s="75"/>
-      <c r="B36" s="76"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="77"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="73"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="75"/>
+    </row>
+    <row r="34" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="76"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="78"/>
+    </row>
+    <row r="35" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="76"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="78"/>
+    </row>
+    <row r="36" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="76"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="78"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="72"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="A29:G29"/>
     <mergeCell ref="A30:G30"/>
@@ -12387,15 +12385,21 @@
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="96" orientation="portrait" r:id="rId1"/>
@@ -12406,24 +12410,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D275738-584E-4BD1-9602-7F4BF70BCF1C}">
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M6:M7"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="14" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
@@ -12455,7 +12460,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -12487,7 +12492,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -12519,7 +12524,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -12539,7 +12544,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -12571,7 +12576,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -12603,7 +12608,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -12623,7 +12628,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -12651,7 +12656,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -12683,7 +12688,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -12703,16 +12708,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="1">
-        <v>165</v>
-      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="52">
         <v>0</v>
       </c>
@@ -12731,16 +12734,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1">
-        <v>165</v>
-      </c>
+      <c r="C12" s="1"/>
       <c r="D12" s="52">
         <v>0</v>
       </c>
@@ -12759,7 +12760,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -12779,16 +12780,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1">
-        <v>165</v>
-      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="52">
         <v>0</v>
       </c>
@@ -12807,16 +12806,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1">
-        <v>165</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="52">
         <v>0</v>
       </c>
@@ -12835,7 +12832,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -12855,16 +12852,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="1">
-        <v>170</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="52">
         <v>0</v>
       </c>
@@ -12883,16 +12878,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="1">
-        <v>175</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="52">
         <v>0</v>
       </c>
@@ -12911,7 +12904,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -12931,16 +12924,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="1">
-        <v>170</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="52">
         <v>0</v>
       </c>
@@ -12959,16 +12950,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="1">
-        <v>175</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="52">
         <v>0</v>
       </c>
@@ -12987,7 +12976,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -13007,16 +12996,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="1">
-        <v>170</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="52">
         <v>0</v>
       </c>
@@ -13035,16 +13022,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="1">
-        <v>175</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="52">
         <v>0</v>
       </c>
@@ -13063,7 +13048,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
@@ -13083,16 +13068,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="1">
-        <v>170</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="52">
         <v>0</v>
       </c>
@@ -13111,16 +13094,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="1">
-        <v>175</v>
-      </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="52">
         <v>0</v>
       </c>
@@ -13139,7 +13120,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>39</v>
       </c>
@@ -13159,7 +13140,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -13191,7 +13172,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -13223,7 +13204,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
@@ -13245,7 +13226,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
@@ -13277,7 +13258,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -13309,7 +13290,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
@@ -13331,7 +13312,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -13363,7 +13344,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>20</v>
       </c>
@@ -13395,7 +13376,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -13417,7 +13398,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
@@ -13449,7 +13430,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -13481,7 +13462,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
@@ -13501,7 +13482,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -13533,7 +13514,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -13565,7 +13546,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -13585,7 +13566,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
@@ -13617,7 +13598,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -13649,7 +13630,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>30</v>
       </c>
@@ -13669,16 +13650,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="34">
-        <v>155</v>
-      </c>
+      <c r="C47" s="34"/>
       <c r="D47" s="1">
         <v>0</v>
       </c>
@@ -13697,16 +13676,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="34">
-        <v>165</v>
-      </c>
+      <c r="C48" s="34"/>
       <c r="D48" s="1">
         <v>0</v>
       </c>
@@ -13725,7 +13702,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
@@ -13745,16 +13722,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B50" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="34">
-        <v>155</v>
-      </c>
+      <c r="C50" s="34"/>
       <c r="D50" s="1">
         <v>0</v>
       </c>
@@ -13773,16 +13748,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B51" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="34">
-        <v>165</v>
-      </c>
+      <c r="C51" s="34"/>
       <c r="D51" s="1">
         <v>0</v>
       </c>
@@ -13801,7 +13774,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>36</v>
       </c>
@@ -13821,16 +13794,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B53" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="34">
-        <v>160</v>
-      </c>
+      <c r="C53" s="34"/>
       <c r="D53" s="1">
         <v>0</v>
       </c>
@@ -13849,16 +13820,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B54" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C54" s="34">
-        <v>170</v>
-      </c>
+      <c r="C54" s="34"/>
       <c r="D54" s="1">
         <v>0</v>
       </c>
@@ -13877,7 +13846,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>39</v>
       </c>
@@ -13897,16 +13866,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B56" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="1">
-        <v>100</v>
-      </c>
+      <c r="C56" s="1"/>
       <c r="D56" s="52">
         <v>0</v>
       </c>
@@ -13925,16 +13892,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B57" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="1">
-        <v>110</v>
-      </c>
+      <c r="C57" s="1"/>
       <c r="D57" s="52">
         <v>0</v>
       </c>
@@ -13953,7 +13918,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>15</v>
       </c>
@@ -13973,7 +13938,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>16</v>
       </c>
@@ -14005,7 +13970,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
@@ -14037,7 +14002,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>18</v>
       </c>
@@ -14057,7 +14022,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>19</v>
       </c>
@@ -14089,7 +14054,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>20</v>
       </c>
@@ -14121,7 +14086,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>21</v>
       </c>
@@ -14141,16 +14106,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B65" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="1">
-        <v>195</v>
-      </c>
+      <c r="C65" s="1"/>
       <c r="D65" s="52">
         <v>0</v>
       </c>
@@ -14169,16 +14132,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B66" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="1">
-        <v>195</v>
-      </c>
+      <c r="C66" s="1"/>
       <c r="D66" s="52">
         <v>0</v>
       </c>
@@ -14197,7 +14158,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>24</v>
       </c>
@@ -14217,16 +14178,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="1">
-        <v>195</v>
-      </c>
+      <c r="C68" s="1"/>
       <c r="D68" s="52">
         <v>0</v>
       </c>
@@ -14245,16 +14204,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B69" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="1">
-        <v>195</v>
-      </c>
+      <c r="C69" s="1"/>
       <c r="D69" s="52">
         <v>0</v>
       </c>
@@ -14273,7 +14230,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>27</v>
       </c>
@@ -14293,16 +14250,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B71" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C71" s="1">
-        <v>200</v>
-      </c>
+      <c r="C71" s="1"/>
       <c r="D71" s="52">
         <v>0</v>
       </c>
@@ -14321,16 +14276,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B72" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C72" s="1">
-        <v>205</v>
-      </c>
+      <c r="C72" s="1"/>
       <c r="D72" s="52">
         <v>0</v>
       </c>
@@ -14349,7 +14302,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>30</v>
       </c>
@@ -14369,7 +14322,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>31</v>
       </c>
@@ -14395,7 +14348,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>32</v>
       </c>
@@ -14421,7 +14374,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>33</v>
       </c>
@@ -14441,7 +14394,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>34</v>
       </c>
@@ -14463,7 +14416,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>35</v>
       </c>
@@ -14485,7 +14438,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>36</v>
       </c>
@@ -14505,7 +14458,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>37</v>
       </c>
@@ -14531,7 +14484,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>38</v>
       </c>
@@ -14557,7 +14510,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>39</v>
       </c>
@@ -14577,7 +14530,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>12</v>
       </c>
@@ -14603,7 +14556,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>14</v>
       </c>
@@ -14629,7 +14582,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>15</v>
       </c>
@@ -14655,7 +14608,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>16</v>
       </c>
@@ -14681,7 +14634,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>17</v>
       </c>
@@ -14713,7 +14666,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>18</v>
       </c>
@@ -14739,7 +14692,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>19</v>
       </c>
@@ -14765,7 +14718,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>20</v>
       </c>
@@ -14791,7 +14744,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>21</v>
       </c>
@@ -14817,7 +14770,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>22</v>
       </c>
@@ -14849,7 +14802,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>23</v>
       </c>
@@ -14881,7 +14834,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>24</v>
       </c>
@@ -14907,7 +14860,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>25</v>
       </c>
@@ -14933,7 +14886,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>26</v>
       </c>
@@ -14959,7 +14912,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>27</v>
       </c>
@@ -14985,7 +14938,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>28</v>
       </c>
@@ -15011,7 +14964,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>29</v>
       </c>
@@ -15037,7 +14990,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>30</v>
       </c>
@@ -15063,7 +15016,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>31</v>
       </c>
@@ -15089,7 +15042,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>32</v>
       </c>
@@ -15115,7 +15068,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>33</v>
       </c>
@@ -15141,7 +15094,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>34</v>
       </c>
@@ -15167,7 +15120,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>35</v>
       </c>
@@ -15193,7 +15146,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>36</v>
       </c>
@@ -15219,7 +15172,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>37</v>
       </c>
@@ -15245,7 +15198,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>38</v>
       </c>
@@ -15271,7 +15224,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>39</v>
       </c>
@@ -15305,6 +15258,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc0df218-5f63-4b1b-aed8-36ec2fc7a699">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7922f4a4-deb7-445d-89c2-4a76bdf9d62e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100729180EC2A42A34E94F6A400BE715B96" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="af5d29db1759d4872da02b1d98af6f46">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dc0df218-5f63-4b1b-aed8-36ec2fc7a699" xmlns:ns3="7922f4a4-deb7-445d-89c2-4a76bdf9d62e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b60febf10e5aa5a1c812767628ccb60" ns2:_="" ns3:_="">
     <xsd:import namespace="dc0df218-5f63-4b1b-aed8-36ec2fc7a699"/>
@@ -15559,34 +15532,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc0df218-5f63-4b1b-aed8-36ec2fc7a699">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7922f4a4-deb7-445d-89c2-4a76bdf9d62e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9886425-7128-404A-9C13-1119769A87B8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9335420-1439-4D70-8E7C-D1EC209BB93C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DDA28A2-8D16-4880-98F0-78A1B73EEC26}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DDA28A2-8D16-4880-98F0-78A1B73EEC26}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc0df218-5f63-4b1b-aed8-36ec2fc7a699"/>
+    <ds:schemaRef ds:uri="7922f4a4-deb7-445d-89c2-4a76bdf9d62e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9335420-1439-4D70-8E7C-D1EC209BB93C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9886425-7128-404A-9C13-1119769A87B8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dc0df218-5f63-4b1b-aed8-36ec2fc7a699"/>
+    <ds:schemaRef ds:uri="7922f4a4-deb7-445d-89c2-4a76bdf9d62e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>